<commit_message>
Updated routine to deal with blanks and multiple values
Added an overall check on the final dimension table to ensure the keys
are still unique.
Added an option to ignore blanks and pick the attribute value when
that is the case (only one value and blank)
Added an option to ignore multiple attributes and pick the first one.
Added sort_values() to the dim table creation, possibly a nice to have
if we are talking millions of records.
Added more print commands to explain what is going on.
</commit_message>
<xml_diff>
--- a/110 star schema/demo_data.xlsx
+++ b/110 star schema/demo_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\paat\110 star schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="13_ncr:1_{13CA5346-4F4A-45FA-A228-271989CFEA6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A291D289-4028-1249-A0D8-7DFE085FBEDE}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{13CA5346-4F4A-45FA-A228-271989CFEA6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{68D386DE-9D04-3C40-BA4E-4A54A39DA70E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="1129">
   <si>
     <t>Country</t>
   </si>
@@ -3391,9 +3391,6 @@
     <t>Radiology</t>
   </si>
   <si>
-    <t>HCA Hospital</t>
-  </si>
-  <si>
     <t>CAT Scans</t>
   </si>
   <si>
@@ -3401,6 +3398,27 @@
   </si>
   <si>
     <t>C08</t>
+  </si>
+  <si>
+    <t>Provider Address</t>
+  </si>
+  <si>
+    <t>San Francisco, CL</t>
+  </si>
+  <si>
+    <t>3 Privet Dr.</t>
+  </si>
+  <si>
+    <t>The Shard, London</t>
+  </si>
+  <si>
+    <t>HCA Clinic</t>
+  </si>
+  <si>
+    <t>1 Kensington Gardens</t>
+  </si>
+  <si>
+    <t>ProviderCountry</t>
   </si>
 </sst>
 </file>
@@ -9345,21 +9363,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D012052-47F4-BB4C-8AF6-45F11B753582}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.296875" customWidth="1"/>
     <col min="3" max="3" width="14.796875" customWidth="1"/>
-    <col min="4" max="8" width="17.890625" customWidth="1"/>
-    <col min="12" max="12" width="12.64453125" customWidth="1"/>
+    <col min="4" max="10" width="17.890625" customWidth="1"/>
+    <col min="14" max="14" width="12.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1084</v>
       </c>
@@ -9373,31 +9391,37 @@
         <v>1082</v>
       </c>
       <c r="E1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G1" t="s">
         <v>1096</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1102</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>1097</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>1098</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>1091</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>1100</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>1101</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>1092</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1085</v>
       </c>
@@ -9410,34 +9434,40 @@
       <c r="D2" t="s">
         <v>1089</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>1103</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>901</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>108</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>1000</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>92</v>
       </c>
-      <c r="K2">
-        <f>VLOOKUP(J2,country_currency!C:G,5,0)</f>
+      <c r="M2">
+        <f>VLOOKUP(L2,country_currency!C:G,5,0)</f>
         <v>1.2767329999999999</v>
       </c>
-      <c r="L2">
-        <f>I2/K2</f>
+      <c r="N2">
+        <f>K2/M2</f>
         <v>783.24912099867402</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1085</v>
       </c>
@@ -9450,34 +9480,40 @@
       <c r="D3" t="s">
         <v>1089</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>1103</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>902</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>108</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>800</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>92</v>
       </c>
-      <c r="K3">
-        <f>VLOOKUP(J3,country_currency!C:G,5,0)</f>
+      <c r="M3">
+        <f>VLOOKUP(L3,country_currency!C:G,5,0)</f>
         <v>1.2767329999999999</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L8" si="0">I3/K3</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="0">K3/M3</f>
         <v>626.59929679893924</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1085</v>
       </c>
@@ -9490,31 +9526,37 @@
       <c r="D4" t="s">
         <v>1090</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G4">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>1104</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>1099</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>400</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>85</v>
       </c>
-      <c r="K4">
-        <f>VLOOKUP(J4,country_currency!C:G,5,0)</f>
+      <c r="M4">
+        <f>VLOOKUP(L4,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1086</v>
       </c>
@@ -9527,34 +9569,40 @@
       <c r="D5" t="s">
         <v>1095</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G5">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>1108</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>501</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>1099</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>200</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>85</v>
       </c>
-      <c r="K5">
-        <f>VLOOKUP(J5,country_currency!C:G,5,0)</f>
+      <c r="M5">
+        <f>VLOOKUP(L5,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1086</v>
       </c>
@@ -9567,34 +9615,40 @@
       <c r="D6" t="s">
         <v>1089</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>1103</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>901</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>108</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>1300</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>92</v>
       </c>
-      <c r="K6">
-        <f>VLOOKUP(J6,country_currency!C:G,5,0)</f>
+      <c r="M6">
+        <f>VLOOKUP(L6,country_currency!C:G,5,0)</f>
         <v>1.2767329999999999</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>1018.2238572982762</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1086</v>
       </c>
@@ -9607,31 +9661,37 @@
       <c r="D7" t="s">
         <v>1090</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G7">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>1104</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>1099</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>300</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>85</v>
       </c>
-      <c r="K7">
-        <f>VLOOKUP(J7,country_currency!C:G,5,0)</f>
+      <c r="M7">
+        <f>VLOOKUP(L7,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1087</v>
       </c>
@@ -9644,31 +9704,37 @@
       <c r="D8" t="s">
         <v>1090</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G8">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>1105</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>1099</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>20</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>85</v>
       </c>
-      <c r="K8">
-        <f>VLOOKUP(J8,country_currency!C:G,5,0)</f>
+      <c r="M8">
+        <f>VLOOKUP(L8,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1087</v>
       </c>
@@ -9681,34 +9747,37 @@
       <c r="D9" t="s">
         <v>1095</v>
       </c>
-      <c r="E9">
+      <c r="F9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G9">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>1108</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>501</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>1099</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>100</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>85</v>
       </c>
-      <c r="K9">
-        <f>VLOOKUP(J9,country_currency!C:G,5,0)</f>
+      <c r="M9">
+        <f>VLOOKUP(L9,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L9">
-        <f t="shared" ref="L9" si="1">I9/K9</f>
+      <c r="N9">
+        <f t="shared" ref="N9" si="1">K9/M9</f>
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1109</v>
       </c>
@@ -9721,34 +9790,40 @@
       <c r="D10" t="s">
         <v>1089</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10">
         <v>10</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>1103</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>903</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>108</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>200</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>92</v>
       </c>
-      <c r="K10">
-        <f>VLOOKUP(J10,country_currency!C:G,5,0)</f>
+      <c r="M10">
+        <f>VLOOKUP(L10,country_currency!C:G,5,0)</f>
         <v>1.2767329999999999</v>
       </c>
-      <c r="L10">
-        <f>I10/K10</f>
+      <c r="N10">
+        <f>K10/M10</f>
         <v>156.64982419973481</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1109</v>
       </c>
@@ -9761,34 +9836,40 @@
       <c r="D11" t="s">
         <v>1089</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>1103</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>902</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>108</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>600</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>92</v>
       </c>
-      <c r="K11">
-        <f>VLOOKUP(J11,country_currency!C:G,5,0)</f>
+      <c r="M11">
+        <f>VLOOKUP(L11,country_currency!C:G,5,0)</f>
         <v>1.2767329999999999</v>
       </c>
-      <c r="L11">
-        <f t="shared" ref="L11:L15" si="2">I11/K11</f>
+      <c r="N11">
+        <f t="shared" ref="N11:N15" si="2">K11/M11</f>
         <v>469.9494725992044</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1111</v>
       </c>
@@ -9801,34 +9882,35 @@
       <c r="D12" t="s">
         <v>1114</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G12">
         <v>40</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>1115</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>100</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>1099</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>500</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>85</v>
       </c>
-      <c r="K12">
-        <f>VLOOKUP(J12,country_currency!C:G,5,0)</f>
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1111</v>
       </c>
@@ -9841,34 +9923,40 @@
       <c r="D13" t="s">
         <v>1114</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G13">
         <v>40</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>1115</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>100</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>1099</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>500</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>85</v>
       </c>
-      <c r="K13">
-        <f>VLOOKUP(J13,country_currency!C:G,5,0)</f>
+      <c r="M13">
+        <f>VLOOKUP(L13,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L13">
-        <f t="shared" ref="L13:L14" si="3">I13/K13</f>
+      <c r="N13">
+        <f t="shared" ref="N13:N14" si="3">K13/M13</f>
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1111</v>
       </c>
@@ -9881,34 +9969,40 @@
       <c r="D14" t="s">
         <v>1114</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G14">
         <v>40</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>1115</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>100</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>1099</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>500</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>85</v>
       </c>
-      <c r="K14">
-        <f>VLOOKUP(J14,country_currency!C:G,5,0)</f>
+      <c r="M14">
+        <f>VLOOKUP(L14,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <f t="shared" si="3"/>
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1111</v>
       </c>
@@ -9919,36 +10013,42 @@
         <v>1116</v>
       </c>
       <c r="D15" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E15">
+        <v>1125</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G15">
         <v>50</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>1117</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>600</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>1099</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>150</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>85</v>
       </c>
-      <c r="K15">
-        <f>VLOOKUP(J15,country_currency!C:G,5,0)</f>
+      <c r="M15">
+        <f>VLOOKUP(L15,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1111</v>
       </c>
@@ -9959,36 +10059,42 @@
         <v>1116</v>
       </c>
       <c r="D16" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s">
         <v>1118</v>
       </c>
-      <c r="E16">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1119</v>
-      </c>
-      <c r="G16">
+      <c r="I16">
         <v>700</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>1099</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>1000</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>85</v>
       </c>
-      <c r="K16">
-        <f>VLOOKUP(J16,country_currency!C:G,5,0)</f>
+      <c r="M16">
+        <f>VLOOKUP(L16,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L16">
-        <f t="shared" ref="L16" si="4">I16/K16</f>
+      <c r="N16">
+        <f t="shared" ref="N16" si="4">K16/M16</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1111</v>
       </c>
@@ -9999,41 +10105,47 @@
         <v>1116</v>
       </c>
       <c r="D17" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E17">
+        <v>1125</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G17">
         <v>80</v>
       </c>
-      <c r="F17" t="s">
-        <v>1120</v>
-      </c>
-      <c r="G17">
+      <c r="H17" t="s">
+        <v>1119</v>
+      </c>
+      <c r="I17">
         <v>810</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>1099</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>1520</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>85</v>
       </c>
-      <c r="K17">
-        <f>VLOOKUP(J17,country_currency!C:G,5,0)</f>
+      <c r="M17">
+        <f>VLOOKUP(L17,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L17">
-        <f t="shared" ref="L17" si="5">I17/K17</f>
+      <c r="N17">
+        <f t="shared" ref="N17" si="5">K17/M17</f>
         <v>1520</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1111</v>
       </c>
       <c r="B18" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C18" t="s">
         <v>1088</v>
@@ -10041,27 +10153,33 @@
       <c r="D18" t="s">
         <v>1090</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G18">
         <v>20</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>1104</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>1099</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>50</v>
       </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>85</v>
       </c>
-      <c r="K18">
-        <f>VLOOKUP(J18,country_currency!C:G,5,0)</f>
+      <c r="M18">
+        <f>VLOOKUP(L18,country_currency!C:G,5,0)</f>
         <v>1</v>
       </c>
-      <c r="L18">
-        <f t="shared" ref="L18" si="6">I18/K18</f>
+      <c r="N18">
+        <f t="shared" ref="N18" si="6">K18/M18</f>
         <v>50</v>
       </c>
     </row>

</xml_diff>